<commit_message>
Scrape new links of Ilca 6 & Ilca 7
</commit_message>
<xml_diff>
--- a/results/World Championship 2017_49er.xlsx
+++ b/results/World Championship 2017_49er.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="59">
   <si>
     <t>Nome Competidor</t>
   </si>
@@ -115,7 +115,10 @@
     <t>10.0</t>
   </si>
   <si>
-    <t>medal</t>
+    <t>G</t>
+  </si>
+  <si>
+    <t>MR</t>
   </si>
   <si>
     <t>UFD</t>
@@ -602,17 +605,20 @@
       <c r="E2">
         <v>0</v>
       </c>
+      <c r="F2" t="s">
+        <v>33</v>
+      </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -631,17 +637,20 @@
       <c r="E3">
         <v>0</v>
       </c>
+      <c r="F3" t="s">
+        <v>33</v>
+      </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -660,17 +669,20 @@
       <c r="E4">
         <v>0</v>
       </c>
+      <c r="F4" t="s">
+        <v>33</v>
+      </c>
       <c r="G4">
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -689,17 +701,20 @@
       <c r="E5">
         <v>0</v>
       </c>
+      <c r="F5" t="s">
+        <v>33</v>
+      </c>
       <c r="G5">
         <v>1</v>
       </c>
       <c r="I5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -718,17 +733,20 @@
       <c r="E6">
         <v>0</v>
       </c>
+      <c r="F6" t="s">
+        <v>33</v>
+      </c>
       <c r="G6">
         <v>1</v>
       </c>
       <c r="I6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -747,17 +765,20 @@
       <c r="E7">
         <v>0</v>
       </c>
+      <c r="F7" t="s">
+        <v>33</v>
+      </c>
       <c r="G7">
         <v>1</v>
       </c>
       <c r="I7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -776,17 +797,20 @@
       <c r="E8">
         <v>0</v>
       </c>
+      <c r="F8" t="s">
+        <v>33</v>
+      </c>
       <c r="G8">
         <v>1</v>
       </c>
       <c r="I8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -805,17 +829,20 @@
       <c r="E9">
         <v>0</v>
       </c>
+      <c r="F9" t="s">
+        <v>33</v>
+      </c>
       <c r="G9">
         <v>1</v>
       </c>
       <c r="I9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -834,17 +861,20 @@
       <c r="E10">
         <v>0</v>
       </c>
+      <c r="F10" t="s">
+        <v>33</v>
+      </c>
       <c r="G10">
         <v>1</v>
       </c>
       <c r="I10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K10" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -863,17 +893,20 @@
       <c r="E11">
         <v>0</v>
       </c>
+      <c r="F11" t="s">
+        <v>33</v>
+      </c>
       <c r="G11">
         <v>1</v>
       </c>
       <c r="I11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J11" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K11" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -892,17 +925,20 @@
       <c r="E12">
         <v>0</v>
       </c>
+      <c r="F12" t="s">
+        <v>33</v>
+      </c>
       <c r="G12">
         <v>1</v>
       </c>
       <c r="I12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J12" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K12" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -921,20 +957,23 @@
       <c r="E13">
         <v>1</v>
       </c>
+      <c r="F13" t="s">
+        <v>33</v>
+      </c>
       <c r="G13">
         <v>1</v>
       </c>
       <c r="H13" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I13" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J13" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K13" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -954,19 +993,19 @@
         <v>0</v>
       </c>
       <c r="F14" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G14">
         <v>1</v>
       </c>
       <c r="I14" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J14" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K14" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -986,19 +1025,19 @@
         <v>0</v>
       </c>
       <c r="F15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G15">
         <v>1</v>
       </c>
       <c r="I15" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J15" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K15" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1018,19 +1057,19 @@
         <v>0</v>
       </c>
       <c r="F16" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G16">
         <v>1</v>
       </c>
       <c r="I16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J16" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K16" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -1049,17 +1088,20 @@
       <c r="E17">
         <v>0</v>
       </c>
+      <c r="F17" t="s">
+        <v>33</v>
+      </c>
       <c r="G17">
         <v>2</v>
       </c>
       <c r="I17" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K17" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -1078,17 +1120,20 @@
       <c r="E18">
         <v>0</v>
       </c>
+      <c r="F18" t="s">
+        <v>33</v>
+      </c>
       <c r="G18">
         <v>2</v>
       </c>
       <c r="I18" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J18" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1107,17 +1152,20 @@
       <c r="E19">
         <v>1</v>
       </c>
+      <c r="F19" t="s">
+        <v>33</v>
+      </c>
       <c r="G19">
         <v>2</v>
       </c>
       <c r="I19" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J19" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K19" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -1136,17 +1184,20 @@
       <c r="E20">
         <v>0</v>
       </c>
+      <c r="F20" t="s">
+        <v>33</v>
+      </c>
       <c r="G20">
         <v>2</v>
       </c>
       <c r="I20" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J20" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K20" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -1165,17 +1216,20 @@
       <c r="E21">
         <v>0</v>
       </c>
+      <c r="F21" t="s">
+        <v>33</v>
+      </c>
       <c r="G21">
         <v>2</v>
       </c>
       <c r="I21" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J21" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K21" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -1194,17 +1248,20 @@
       <c r="E22">
         <v>0</v>
       </c>
+      <c r="F22" t="s">
+        <v>33</v>
+      </c>
       <c r="G22">
         <v>2</v>
       </c>
       <c r="I22" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J22" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K22" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -1223,17 +1280,20 @@
       <c r="E23">
         <v>0</v>
       </c>
+      <c r="F23" t="s">
+        <v>33</v>
+      </c>
       <c r="G23">
         <v>2</v>
       </c>
       <c r="I23" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J23" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K23" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -1252,20 +1312,23 @@
       <c r="E24">
         <v>0</v>
       </c>
+      <c r="F24" t="s">
+        <v>33</v>
+      </c>
       <c r="G24">
         <v>2</v>
       </c>
       <c r="H24" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I24" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J24" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K24" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -1284,17 +1347,20 @@
       <c r="E25">
         <v>0</v>
       </c>
+      <c r="F25" t="s">
+        <v>33</v>
+      </c>
       <c r="G25">
         <v>2</v>
       </c>
       <c r="I25" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J25" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K25" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -1313,17 +1379,20 @@
       <c r="E26">
         <v>0</v>
       </c>
+      <c r="F26" t="s">
+        <v>33</v>
+      </c>
       <c r="G26">
         <v>2</v>
       </c>
       <c r="I26" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J26" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K26" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -1342,17 +1411,20 @@
       <c r="E27">
         <v>0</v>
       </c>
+      <c r="F27" t="s">
+        <v>33</v>
+      </c>
       <c r="G27">
         <v>2</v>
       </c>
       <c r="I27" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J27" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K27" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -1371,17 +1443,20 @@
       <c r="E28">
         <v>0</v>
       </c>
+      <c r="F28" t="s">
+        <v>33</v>
+      </c>
       <c r="G28">
         <v>2</v>
       </c>
       <c r="I28" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J28" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K28" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -1401,19 +1476,19 @@
         <v>0</v>
       </c>
       <c r="F29" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G29">
         <v>2</v>
       </c>
       <c r="I29" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J29" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K29" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -1433,19 +1508,19 @@
         <v>0</v>
       </c>
       <c r="F30" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G30">
         <v>2</v>
       </c>
       <c r="I30" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J30" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K30" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -1465,19 +1540,19 @@
         <v>0</v>
       </c>
       <c r="F31" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G31">
         <v>2</v>
       </c>
       <c r="I31" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J31" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K31" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="32" spans="1:11">
@@ -1496,17 +1571,20 @@
       <c r="E32">
         <v>0</v>
       </c>
+      <c r="F32" t="s">
+        <v>33</v>
+      </c>
       <c r="G32">
         <v>3</v>
       </c>
       <c r="I32" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J32" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K32" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="33" spans="1:11">
@@ -1525,17 +1603,20 @@
       <c r="E33">
         <v>0</v>
       </c>
+      <c r="F33" t="s">
+        <v>33</v>
+      </c>
       <c r="G33">
         <v>3</v>
       </c>
       <c r="I33" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J33" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K33" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:11">
@@ -1554,17 +1635,20 @@
       <c r="E34">
         <v>0</v>
       </c>
+      <c r="F34" t="s">
+        <v>33</v>
+      </c>
       <c r="G34">
         <v>3</v>
       </c>
       <c r="I34" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J34" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K34" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="35" spans="1:11">
@@ -1583,17 +1667,20 @@
       <c r="E35">
         <v>0</v>
       </c>
+      <c r="F35" t="s">
+        <v>33</v>
+      </c>
       <c r="G35">
         <v>3</v>
       </c>
       <c r="I35" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J35" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K35" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="36" spans="1:11">
@@ -1612,17 +1699,20 @@
       <c r="E36">
         <v>0</v>
       </c>
+      <c r="F36" t="s">
+        <v>33</v>
+      </c>
       <c r="G36">
         <v>3</v>
       </c>
       <c r="I36" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J36" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K36" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="37" spans="1:11">
@@ -1641,17 +1731,20 @@
       <c r="E37">
         <v>0</v>
       </c>
+      <c r="F37" t="s">
+        <v>33</v>
+      </c>
       <c r="G37">
         <v>3</v>
       </c>
       <c r="I37" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J37" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K37" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="38" spans="1:11">
@@ -1670,17 +1763,20 @@
       <c r="E38">
         <v>0</v>
       </c>
+      <c r="F38" t="s">
+        <v>33</v>
+      </c>
       <c r="G38">
         <v>3</v>
       </c>
       <c r="I38" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J38" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K38" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="39" spans="1:11">
@@ -1699,17 +1795,20 @@
       <c r="E39">
         <v>0</v>
       </c>
+      <c r="F39" t="s">
+        <v>33</v>
+      </c>
       <c r="G39">
         <v>3</v>
       </c>
       <c r="I39" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J39" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K39" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:11">
@@ -1728,17 +1827,20 @@
       <c r="E40">
         <v>0</v>
       </c>
+      <c r="F40" t="s">
+        <v>33</v>
+      </c>
       <c r="G40">
         <v>3</v>
       </c>
       <c r="I40" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J40" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K40" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="41" spans="1:11">
@@ -1757,17 +1859,20 @@
       <c r="E41">
         <v>1</v>
       </c>
+      <c r="F41" t="s">
+        <v>33</v>
+      </c>
       <c r="G41">
         <v>3</v>
       </c>
       <c r="I41" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J41" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K41" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="42" spans="1:11">
@@ -1786,17 +1891,20 @@
       <c r="E42">
         <v>0</v>
       </c>
+      <c r="F42" t="s">
+        <v>33</v>
+      </c>
       <c r="G42">
         <v>3</v>
       </c>
       <c r="I42" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J42" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K42" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="43" spans="1:11">
@@ -1815,17 +1923,20 @@
       <c r="E43">
         <v>0</v>
       </c>
+      <c r="F43" t="s">
+        <v>33</v>
+      </c>
       <c r="G43">
         <v>3</v>
       </c>
       <c r="I43" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J43" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K43" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="44" spans="1:11">
@@ -1845,19 +1956,19 @@
         <v>0</v>
       </c>
       <c r="F44" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G44">
         <v>3</v>
       </c>
       <c r="I44" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J44" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K44" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="45" spans="1:11">
@@ -1877,19 +1988,19 @@
         <v>0</v>
       </c>
       <c r="F45" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G45">
         <v>3</v>
       </c>
       <c r="I45" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J45" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K45" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="46" spans="1:11">
@@ -1909,19 +2020,19 @@
         <v>0</v>
       </c>
       <c r="F46" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G46">
         <v>3</v>
       </c>
       <c r="I46" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J46" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K46" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="47" spans="1:11">
@@ -1940,17 +2051,20 @@
       <c r="E47">
         <v>0</v>
       </c>
+      <c r="F47" t="s">
+        <v>33</v>
+      </c>
       <c r="G47">
         <v>4</v>
       </c>
       <c r="I47" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J47" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K47" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="48" spans="1:11">
@@ -1969,17 +2083,20 @@
       <c r="E48">
         <v>0</v>
       </c>
+      <c r="F48" t="s">
+        <v>33</v>
+      </c>
       <c r="G48">
         <v>4</v>
       </c>
       <c r="I48" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J48" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K48" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="49" spans="1:11">
@@ -1998,17 +2115,20 @@
       <c r="E49">
         <v>1</v>
       </c>
+      <c r="F49" t="s">
+        <v>33</v>
+      </c>
       <c r="G49">
         <v>4</v>
       </c>
       <c r="I49" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J49" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K49" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="50" spans="1:11">
@@ -2027,17 +2147,20 @@
       <c r="E50">
         <v>0</v>
       </c>
+      <c r="F50" t="s">
+        <v>33</v>
+      </c>
       <c r="G50">
         <v>4</v>
       </c>
       <c r="I50" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J50" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K50" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="51" spans="1:11">
@@ -2056,17 +2179,20 @@
       <c r="E51">
         <v>0</v>
       </c>
+      <c r="F51" t="s">
+        <v>33</v>
+      </c>
       <c r="G51">
         <v>4</v>
       </c>
       <c r="I51" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J51" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K51" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="52" spans="1:11">
@@ -2085,17 +2211,20 @@
       <c r="E52">
         <v>0</v>
       </c>
+      <c r="F52" t="s">
+        <v>33</v>
+      </c>
       <c r="G52">
         <v>4</v>
       </c>
       <c r="I52" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J52" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K52" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="53" spans="1:11">
@@ -2114,17 +2243,20 @@
       <c r="E53">
         <v>0</v>
       </c>
+      <c r="F53" t="s">
+        <v>33</v>
+      </c>
       <c r="G53">
         <v>4</v>
       </c>
       <c r="I53" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J53" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K53" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="54" spans="1:11">
@@ -2143,17 +2275,20 @@
       <c r="E54">
         <v>0</v>
       </c>
+      <c r="F54" t="s">
+        <v>33</v>
+      </c>
       <c r="G54">
         <v>4</v>
       </c>
       <c r="I54" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J54" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K54" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="55" spans="1:11">
@@ -2172,17 +2307,20 @@
       <c r="E55">
         <v>0</v>
       </c>
+      <c r="F55" t="s">
+        <v>33</v>
+      </c>
       <c r="G55">
         <v>4</v>
       </c>
       <c r="I55" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J55" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K55" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="56" spans="1:11">
@@ -2201,17 +2339,20 @@
       <c r="E56">
         <v>0</v>
       </c>
+      <c r="F56" t="s">
+        <v>33</v>
+      </c>
       <c r="G56">
         <v>4</v>
       </c>
       <c r="I56" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J56" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K56" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="57" spans="1:11">
@@ -2230,17 +2371,20 @@
       <c r="E57">
         <v>0</v>
       </c>
+      <c r="F57" t="s">
+        <v>33</v>
+      </c>
       <c r="G57">
         <v>4</v>
       </c>
       <c r="I57" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J57" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K57" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="58" spans="1:11">
@@ -2259,17 +2403,20 @@
       <c r="E58">
         <v>0</v>
       </c>
+      <c r="F58" t="s">
+        <v>33</v>
+      </c>
       <c r="G58">
         <v>4</v>
       </c>
       <c r="I58" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J58" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K58" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="59" spans="1:11">
@@ -2289,19 +2436,19 @@
         <v>0</v>
       </c>
       <c r="F59" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G59">
         <v>4</v>
       </c>
       <c r="I59" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J59" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K59" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="60" spans="1:11">
@@ -2321,19 +2468,19 @@
         <v>0</v>
       </c>
       <c r="F60" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G60">
         <v>4</v>
       </c>
       <c r="I60" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J60" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K60" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="61" spans="1:11">
@@ -2353,19 +2500,19 @@
         <v>0</v>
       </c>
       <c r="F61" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G61">
         <v>4</v>
       </c>
       <c r="I61" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J61" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K61" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="62" spans="1:11">
@@ -2384,17 +2531,20 @@
       <c r="E62">
         <v>0</v>
       </c>
+      <c r="F62" t="s">
+        <v>33</v>
+      </c>
       <c r="G62">
         <v>5</v>
       </c>
       <c r="I62" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J62" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K62" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="63" spans="1:11">
@@ -2413,17 +2563,20 @@
       <c r="E63">
         <v>1</v>
       </c>
+      <c r="F63" t="s">
+        <v>33</v>
+      </c>
       <c r="G63">
         <v>5</v>
       </c>
       <c r="I63" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J63" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K63" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="64" spans="1:11">
@@ -2442,17 +2595,20 @@
       <c r="E64">
         <v>0</v>
       </c>
+      <c r="F64" t="s">
+        <v>33</v>
+      </c>
       <c r="G64">
         <v>5</v>
       </c>
       <c r="I64" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J64" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K64" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="65" spans="1:11">
@@ -2471,17 +2627,20 @@
       <c r="E65">
         <v>0</v>
       </c>
+      <c r="F65" t="s">
+        <v>33</v>
+      </c>
       <c r="G65">
         <v>5</v>
       </c>
       <c r="I65" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J65" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K65" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="66" spans="1:11">
@@ -2500,17 +2659,20 @@
       <c r="E66">
         <v>0</v>
       </c>
+      <c r="F66" t="s">
+        <v>33</v>
+      </c>
       <c r="G66">
         <v>5</v>
       </c>
       <c r="I66" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J66" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K66" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="67" spans="1:11">
@@ -2529,17 +2691,20 @@
       <c r="E67">
         <v>0</v>
       </c>
+      <c r="F67" t="s">
+        <v>33</v>
+      </c>
       <c r="G67">
         <v>5</v>
       </c>
       <c r="I67" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J67" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K67" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="68" spans="1:11">
@@ -2558,17 +2723,20 @@
       <c r="E68">
         <v>0</v>
       </c>
+      <c r="F68" t="s">
+        <v>33</v>
+      </c>
       <c r="G68">
         <v>5</v>
       </c>
       <c r="I68" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J68" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K68" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="69" spans="1:11">
@@ -2587,17 +2755,20 @@
       <c r="E69">
         <v>0</v>
       </c>
+      <c r="F69" t="s">
+        <v>33</v>
+      </c>
       <c r="G69">
         <v>5</v>
       </c>
       <c r="I69" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J69" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K69" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="70" spans="1:11">
@@ -2616,17 +2787,20 @@
       <c r="E70">
         <v>0</v>
       </c>
+      <c r="F70" t="s">
+        <v>33</v>
+      </c>
       <c r="G70">
         <v>5</v>
       </c>
       <c r="I70" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J70" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K70" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="71" spans="1:11">
@@ -2645,17 +2819,20 @@
       <c r="E71">
         <v>0</v>
       </c>
+      <c r="F71" t="s">
+        <v>33</v>
+      </c>
       <c r="G71">
         <v>5</v>
       </c>
       <c r="I71" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J71" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K71" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="72" spans="1:11">
@@ -2674,17 +2851,20 @@
       <c r="E72">
         <v>0</v>
       </c>
+      <c r="F72" t="s">
+        <v>33</v>
+      </c>
       <c r="G72">
         <v>5</v>
       </c>
       <c r="I72" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J72" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K72" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="73" spans="1:11">
@@ -2703,17 +2883,20 @@
       <c r="E73">
         <v>0</v>
       </c>
+      <c r="F73" t="s">
+        <v>33</v>
+      </c>
       <c r="G73">
         <v>5</v>
       </c>
       <c r="I73" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J73" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K73" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="74" spans="1:11">
@@ -2733,19 +2916,19 @@
         <v>0</v>
       </c>
       <c r="F74" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G74">
         <v>5</v>
       </c>
       <c r="I74" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J74" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K74" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="75" spans="1:11">
@@ -2765,19 +2948,19 @@
         <v>0</v>
       </c>
       <c r="F75" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G75">
         <v>5</v>
       </c>
       <c r="I75" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J75" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K75" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="76" spans="1:11">
@@ -2797,19 +2980,19 @@
         <v>0</v>
       </c>
       <c r="F76" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G76">
         <v>5</v>
       </c>
       <c r="I76" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J76" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K76" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="77" spans="1:11">
@@ -2828,17 +3011,20 @@
       <c r="E77">
         <v>0</v>
       </c>
+      <c r="F77" t="s">
+        <v>33</v>
+      </c>
       <c r="G77">
         <v>6</v>
       </c>
       <c r="I77" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J77" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K77" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="78" spans="1:11">
@@ -2857,17 +3043,20 @@
       <c r="E78">
         <v>0</v>
       </c>
+      <c r="F78" t="s">
+        <v>33</v>
+      </c>
       <c r="G78">
         <v>6</v>
       </c>
       <c r="I78" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J78" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K78" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="79" spans="1:11">
@@ -2886,17 +3075,20 @@
       <c r="E79">
         <v>0</v>
       </c>
+      <c r="F79" t="s">
+        <v>33</v>
+      </c>
       <c r="G79">
         <v>6</v>
       </c>
       <c r="I79" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J79" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K79" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="80" spans="1:11">
@@ -2915,17 +3107,20 @@
       <c r="E80">
         <v>0</v>
       </c>
+      <c r="F80" t="s">
+        <v>33</v>
+      </c>
       <c r="G80">
         <v>6</v>
       </c>
       <c r="I80" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J80" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K80" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="81" spans="1:11">
@@ -2944,17 +3139,20 @@
       <c r="E81">
         <v>0</v>
       </c>
+      <c r="F81" t="s">
+        <v>33</v>
+      </c>
       <c r="G81">
         <v>6</v>
       </c>
       <c r="I81" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J81" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K81" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="82" spans="1:11">
@@ -2973,17 +3171,20 @@
       <c r="E82">
         <v>0</v>
       </c>
+      <c r="F82" t="s">
+        <v>33</v>
+      </c>
       <c r="G82">
         <v>6</v>
       </c>
       <c r="I82" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J82" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K82" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="83" spans="1:11">
@@ -3002,17 +3203,20 @@
       <c r="E83">
         <v>1</v>
       </c>
+      <c r="F83" t="s">
+        <v>33</v>
+      </c>
       <c r="G83">
         <v>6</v>
       </c>
       <c r="I83" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J83" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K83" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="84" spans="1:11">
@@ -3031,17 +3235,20 @@
       <c r="E84">
         <v>0</v>
       </c>
+      <c r="F84" t="s">
+        <v>33</v>
+      </c>
       <c r="G84">
         <v>6</v>
       </c>
       <c r="I84" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J84" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K84" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="85" spans="1:11">
@@ -3060,17 +3267,20 @@
       <c r="E85">
         <v>0</v>
       </c>
+      <c r="F85" t="s">
+        <v>33</v>
+      </c>
       <c r="G85">
         <v>6</v>
       </c>
       <c r="I85" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J85" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K85" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="86" spans="1:11">
@@ -3089,17 +3299,20 @@
       <c r="E86">
         <v>0</v>
       </c>
+      <c r="F86" t="s">
+        <v>33</v>
+      </c>
       <c r="G86">
         <v>6</v>
       </c>
       <c r="I86" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J86" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K86" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="87" spans="1:11">
@@ -3118,17 +3331,20 @@
       <c r="E87">
         <v>0</v>
       </c>
+      <c r="F87" t="s">
+        <v>33</v>
+      </c>
       <c r="G87">
         <v>6</v>
       </c>
       <c r="I87" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J87" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K87" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="88" spans="1:11">
@@ -3147,17 +3363,20 @@
       <c r="E88">
         <v>0</v>
       </c>
+      <c r="F88" t="s">
+        <v>33</v>
+      </c>
       <c r="G88">
         <v>6</v>
       </c>
       <c r="I88" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J88" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K88" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="89" spans="1:11">
@@ -3177,22 +3396,22 @@
         <v>0</v>
       </c>
       <c r="F89" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G89">
         <v>6</v>
       </c>
       <c r="H89" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I89" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J89" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K89" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="90" spans="1:11">
@@ -3212,19 +3431,19 @@
         <v>0</v>
       </c>
       <c r="F90" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G90">
         <v>6</v>
       </c>
       <c r="I90" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J90" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K90" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="91" spans="1:11">
@@ -3244,19 +3463,19 @@
         <v>0</v>
       </c>
       <c r="F91" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G91">
         <v>6</v>
       </c>
       <c r="I91" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J91" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K91" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="92" spans="1:11">
@@ -3275,17 +3494,20 @@
       <c r="E92">
         <v>0</v>
       </c>
+      <c r="F92" t="s">
+        <v>33</v>
+      </c>
       <c r="G92">
         <v>7</v>
       </c>
       <c r="I92" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J92" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="K92" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="93" spans="1:11">
@@ -3304,17 +3526,20 @@
       <c r="E93">
         <v>0</v>
       </c>
+      <c r="F93" t="s">
+        <v>33</v>
+      </c>
       <c r="G93">
         <v>7</v>
       </c>
       <c r="I93" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J93" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="K93" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="94" spans="1:11">
@@ -3333,17 +3558,20 @@
       <c r="E94">
         <v>0</v>
       </c>
+      <c r="F94" t="s">
+        <v>33</v>
+      </c>
       <c r="G94">
         <v>7</v>
       </c>
       <c r="I94" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J94" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="K94" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="95" spans="1:11">
@@ -3362,20 +3590,23 @@
       <c r="E95">
         <v>1</v>
       </c>
+      <c r="F95" t="s">
+        <v>33</v>
+      </c>
       <c r="G95">
         <v>7</v>
       </c>
       <c r="H95" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I95" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J95" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="K95" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="96" spans="1:11">
@@ -3394,17 +3625,20 @@
       <c r="E96">
         <v>0</v>
       </c>
+      <c r="F96" t="s">
+        <v>33</v>
+      </c>
       <c r="G96">
         <v>7</v>
       </c>
       <c r="I96" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J96" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="K96" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="97" spans="1:11">
@@ -3423,17 +3657,20 @@
       <c r="E97">
         <v>0</v>
       </c>
+      <c r="F97" t="s">
+        <v>33</v>
+      </c>
       <c r="G97">
         <v>7</v>
       </c>
       <c r="I97" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J97" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="K97" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="98" spans="1:11">
@@ -3452,17 +3689,20 @@
       <c r="E98">
         <v>0</v>
       </c>
+      <c r="F98" t="s">
+        <v>33</v>
+      </c>
       <c r="G98">
         <v>7</v>
       </c>
       <c r="I98" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J98" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="K98" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="99" spans="1:11">
@@ -3481,17 +3721,20 @@
       <c r="E99">
         <v>0</v>
       </c>
+      <c r="F99" t="s">
+        <v>33</v>
+      </c>
       <c r="G99">
         <v>7</v>
       </c>
       <c r="I99" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J99" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="K99" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="100" spans="1:11">
@@ -3510,17 +3753,20 @@
       <c r="E100">
         <v>0</v>
       </c>
+      <c r="F100" t="s">
+        <v>33</v>
+      </c>
       <c r="G100">
         <v>7</v>
       </c>
       <c r="I100" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J100" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="K100" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="101" spans="1:11">
@@ -3539,17 +3785,20 @@
       <c r="E101">
         <v>0</v>
       </c>
+      <c r="F101" t="s">
+        <v>33</v>
+      </c>
       <c r="G101">
         <v>7</v>
       </c>
       <c r="I101" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J101" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="K101" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="102" spans="1:11">
@@ -3568,17 +3817,20 @@
       <c r="E102">
         <v>0</v>
       </c>
+      <c r="F102" t="s">
+        <v>33</v>
+      </c>
       <c r="G102">
         <v>7</v>
       </c>
       <c r="I102" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J102" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="K102" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="103" spans="1:11">
@@ -3597,17 +3849,20 @@
       <c r="E103">
         <v>0</v>
       </c>
+      <c r="F103" t="s">
+        <v>33</v>
+      </c>
       <c r="G103">
         <v>7</v>
       </c>
       <c r="I103" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J103" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="K103" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="104" spans="1:11">
@@ -3627,19 +3882,19 @@
         <v>0</v>
       </c>
       <c r="F104" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G104">
         <v>7</v>
       </c>
       <c r="I104" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J104" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="K104" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="105" spans="1:11">
@@ -3659,19 +3914,19 @@
         <v>0</v>
       </c>
       <c r="F105" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G105">
         <v>7</v>
       </c>
       <c r="I105" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J105" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="K105" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="106" spans="1:11">
@@ -3691,19 +3946,19 @@
         <v>0</v>
       </c>
       <c r="F106" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G106">
         <v>7</v>
       </c>
       <c r="I106" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J106" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="K106" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="107" spans="1:11">
@@ -3722,17 +3977,20 @@
       <c r="E107">
         <v>0</v>
       </c>
+      <c r="F107" t="s">
+        <v>33</v>
+      </c>
       <c r="G107">
         <v>8</v>
       </c>
       <c r="I107" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J107" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K107" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="108" spans="1:11">
@@ -3751,17 +4009,20 @@
       <c r="E108">
         <v>0</v>
       </c>
+      <c r="F108" t="s">
+        <v>33</v>
+      </c>
       <c r="G108">
         <v>8</v>
       </c>
       <c r="I108" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J108" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K108" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="109" spans="1:11">
@@ -3780,17 +4041,20 @@
       <c r="E109">
         <v>0</v>
       </c>
+      <c r="F109" t="s">
+        <v>33</v>
+      </c>
       <c r="G109">
         <v>8</v>
       </c>
       <c r="I109" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J109" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K109" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="110" spans="1:11">
@@ -3809,20 +4073,23 @@
       <c r="E110">
         <v>1</v>
       </c>
+      <c r="F110" t="s">
+        <v>33</v>
+      </c>
       <c r="G110">
         <v>8</v>
       </c>
       <c r="H110" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I110" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J110" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K110" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="111" spans="1:11">
@@ -3841,17 +4108,20 @@
       <c r="E111">
         <v>0</v>
       </c>
+      <c r="F111" t="s">
+        <v>33</v>
+      </c>
       <c r="G111">
         <v>8</v>
       </c>
       <c r="I111" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J111" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K111" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="112" spans="1:11">
@@ -3870,17 +4140,20 @@
       <c r="E112">
         <v>0</v>
       </c>
+      <c r="F112" t="s">
+        <v>33</v>
+      </c>
       <c r="G112">
         <v>8</v>
       </c>
       <c r="I112" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J112" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K112" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="113" spans="1:11">
@@ -3899,17 +4172,20 @@
       <c r="E113">
         <v>0</v>
       </c>
+      <c r="F113" t="s">
+        <v>33</v>
+      </c>
       <c r="G113">
         <v>8</v>
       </c>
       <c r="I113" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J113" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K113" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="114" spans="1:11">
@@ -3928,17 +4204,20 @@
       <c r="E114">
         <v>0</v>
       </c>
+      <c r="F114" t="s">
+        <v>33</v>
+      </c>
       <c r="G114">
         <v>8</v>
       </c>
       <c r="I114" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J114" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K114" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="115" spans="1:11">
@@ -3957,17 +4236,20 @@
       <c r="E115">
         <v>0</v>
       </c>
+      <c r="F115" t="s">
+        <v>33</v>
+      </c>
       <c r="G115">
         <v>8</v>
       </c>
       <c r="I115" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J115" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K115" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="116" spans="1:11">
@@ -3986,17 +4268,20 @@
       <c r="E116">
         <v>0</v>
       </c>
+      <c r="F116" t="s">
+        <v>33</v>
+      </c>
       <c r="G116">
         <v>8</v>
       </c>
       <c r="I116" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J116" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K116" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="117" spans="1:11">
@@ -4015,17 +4300,20 @@
       <c r="E117">
         <v>0</v>
       </c>
+      <c r="F117" t="s">
+        <v>33</v>
+      </c>
       <c r="G117">
         <v>8</v>
       </c>
       <c r="I117" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J117" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K117" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="118" spans="1:11">
@@ -4044,17 +4332,20 @@
       <c r="E118">
         <v>0</v>
       </c>
+      <c r="F118" t="s">
+        <v>33</v>
+      </c>
       <c r="G118">
         <v>8</v>
       </c>
       <c r="I118" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J118" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K118" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="119" spans="1:11">
@@ -4074,19 +4365,19 @@
         <v>0</v>
       </c>
       <c r="F119" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G119">
         <v>8</v>
       </c>
       <c r="I119" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J119" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K119" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="120" spans="1:11">
@@ -4106,19 +4397,19 @@
         <v>0</v>
       </c>
       <c r="F120" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G120">
         <v>8</v>
       </c>
       <c r="I120" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J120" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K120" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="121" spans="1:11">
@@ -4138,19 +4429,19 @@
         <v>0</v>
       </c>
       <c r="F121" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G121">
         <v>8</v>
       </c>
       <c r="I121" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J121" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K121" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="122" spans="1:11">
@@ -4169,17 +4460,20 @@
       <c r="E122">
         <v>0</v>
       </c>
+      <c r="F122" t="s">
+        <v>33</v>
+      </c>
       <c r="G122">
         <v>9</v>
       </c>
       <c r="I122" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J122" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="K122" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="123" spans="1:11">
@@ -4198,17 +4492,20 @@
       <c r="E123">
         <v>0</v>
       </c>
+      <c r="F123" t="s">
+        <v>33</v>
+      </c>
       <c r="G123">
         <v>9</v>
       </c>
       <c r="I123" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J123" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="K123" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="124" spans="1:11">
@@ -4227,17 +4524,20 @@
       <c r="E124">
         <v>0</v>
       </c>
+      <c r="F124" t="s">
+        <v>33</v>
+      </c>
       <c r="G124">
         <v>9</v>
       </c>
       <c r="I124" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J124" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="K124" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="125" spans="1:11">
@@ -4256,17 +4556,20 @@
       <c r="E125">
         <v>0</v>
       </c>
+      <c r="F125" t="s">
+        <v>33</v>
+      </c>
       <c r="G125">
         <v>9</v>
       </c>
       <c r="I125" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J125" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="K125" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="126" spans="1:11">
@@ -4285,17 +4588,20 @@
       <c r="E126">
         <v>0</v>
       </c>
+      <c r="F126" t="s">
+        <v>33</v>
+      </c>
       <c r="G126">
         <v>9</v>
       </c>
       <c r="I126" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J126" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="K126" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="127" spans="1:11">
@@ -4314,17 +4620,20 @@
       <c r="E127">
         <v>0</v>
       </c>
+      <c r="F127" t="s">
+        <v>33</v>
+      </c>
       <c r="G127">
         <v>9</v>
       </c>
       <c r="I127" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J127" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="K127" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="128" spans="1:11">
@@ -4343,17 +4652,20 @@
       <c r="E128">
         <v>0</v>
       </c>
+      <c r="F128" t="s">
+        <v>33</v>
+      </c>
       <c r="G128">
         <v>9</v>
       </c>
       <c r="I128" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J128" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="K128" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="129" spans="1:11">
@@ -4372,17 +4684,20 @@
       <c r="E129">
         <v>0</v>
       </c>
+      <c r="F129" t="s">
+        <v>33</v>
+      </c>
       <c r="G129">
         <v>9</v>
       </c>
       <c r="I129" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J129" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="K129" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="130" spans="1:11">
@@ -4401,17 +4716,20 @@
       <c r="E130">
         <v>0</v>
       </c>
+      <c r="F130" t="s">
+        <v>33</v>
+      </c>
       <c r="G130">
         <v>9</v>
       </c>
       <c r="I130" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J130" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="K130" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="131" spans="1:11">
@@ -4430,17 +4748,20 @@
       <c r="E131">
         <v>0</v>
       </c>
+      <c r="F131" t="s">
+        <v>33</v>
+      </c>
       <c r="G131">
         <v>9</v>
       </c>
       <c r="I131" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J131" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="K131" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="132" spans="1:11">
@@ -4459,20 +4780,23 @@
       <c r="E132">
         <v>1</v>
       </c>
+      <c r="F132" t="s">
+        <v>33</v>
+      </c>
       <c r="G132">
         <v>9</v>
       </c>
       <c r="H132" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I132" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J132" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="K132" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="133" spans="1:11">
@@ -4491,17 +4815,20 @@
       <c r="E133">
         <v>0</v>
       </c>
+      <c r="F133" t="s">
+        <v>33</v>
+      </c>
       <c r="G133">
         <v>9</v>
       </c>
       <c r="I133" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J133" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="K133" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="134" spans="1:11">
@@ -4521,19 +4848,19 @@
         <v>0</v>
       </c>
       <c r="F134" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G134">
         <v>9</v>
       </c>
       <c r="I134" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J134" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="K134" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="135" spans="1:11">
@@ -4553,19 +4880,19 @@
         <v>0</v>
       </c>
       <c r="F135" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G135">
         <v>9</v>
       </c>
       <c r="I135" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J135" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="K135" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="136" spans="1:11">
@@ -4585,19 +4912,19 @@
         <v>0</v>
       </c>
       <c r="F136" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G136">
         <v>9</v>
       </c>
       <c r="I136" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J136" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="K136" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="137" spans="1:11">
@@ -4616,17 +4943,20 @@
       <c r="E137">
         <v>0</v>
       </c>
+      <c r="F137" t="s">
+        <v>33</v>
+      </c>
       <c r="G137">
         <v>10</v>
       </c>
       <c r="I137" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J137" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="K137" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="138" spans="1:11">
@@ -4645,20 +4975,23 @@
       <c r="E138">
         <v>1</v>
       </c>
+      <c r="F138" t="s">
+        <v>33</v>
+      </c>
       <c r="G138">
         <v>10</v>
       </c>
       <c r="H138" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I138" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J138" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="K138" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="139" spans="1:11">
@@ -4677,17 +5010,20 @@
       <c r="E139">
         <v>0</v>
       </c>
+      <c r="F139" t="s">
+        <v>33</v>
+      </c>
       <c r="G139">
         <v>10</v>
       </c>
       <c r="I139" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J139" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="K139" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="140" spans="1:11">
@@ -4706,17 +5042,20 @@
       <c r="E140">
         <v>0</v>
       </c>
+      <c r="F140" t="s">
+        <v>33</v>
+      </c>
       <c r="G140">
         <v>10</v>
       </c>
       <c r="I140" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J140" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="K140" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="141" spans="1:11">
@@ -4735,17 +5074,20 @@
       <c r="E141">
         <v>0</v>
       </c>
+      <c r="F141" t="s">
+        <v>33</v>
+      </c>
       <c r="G141">
         <v>10</v>
       </c>
       <c r="I141" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J141" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="K141" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="142" spans="1:11">
@@ -4764,17 +5106,20 @@
       <c r="E142">
         <v>0</v>
       </c>
+      <c r="F142" t="s">
+        <v>33</v>
+      </c>
       <c r="G142">
         <v>10</v>
       </c>
       <c r="I142" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J142" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="K142" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="143" spans="1:11">
@@ -4793,17 +5138,20 @@
       <c r="E143">
         <v>0</v>
       </c>
+      <c r="F143" t="s">
+        <v>33</v>
+      </c>
       <c r="G143">
         <v>10</v>
       </c>
       <c r="I143" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J143" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="K143" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="144" spans="1:11">
@@ -4822,17 +5170,20 @@
       <c r="E144">
         <v>0</v>
       </c>
+      <c r="F144" t="s">
+        <v>33</v>
+      </c>
       <c r="G144">
         <v>10</v>
       </c>
       <c r="I144" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J144" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="K144" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="145" spans="1:11">
@@ -4851,20 +5202,23 @@
       <c r="E145">
         <v>0</v>
       </c>
+      <c r="F145" t="s">
+        <v>33</v>
+      </c>
       <c r="G145">
         <v>10</v>
       </c>
       <c r="H145" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I145" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J145" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="K145" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="146" spans="1:11">
@@ -4883,17 +5237,20 @@
       <c r="E146">
         <v>0</v>
       </c>
+      <c r="F146" t="s">
+        <v>33</v>
+      </c>
       <c r="G146">
         <v>10</v>
       </c>
       <c r="I146" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J146" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="K146" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="147" spans="1:11">
@@ -4912,17 +5269,20 @@
       <c r="E147">
         <v>0</v>
       </c>
+      <c r="F147" t="s">
+        <v>33</v>
+      </c>
       <c r="G147">
         <v>10</v>
       </c>
       <c r="I147" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J147" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="K147" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="148" spans="1:11">
@@ -4941,17 +5301,20 @@
       <c r="E148">
         <v>0</v>
       </c>
+      <c r="F148" t="s">
+        <v>33</v>
+      </c>
       <c r="G148">
         <v>10</v>
       </c>
       <c r="I148" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J148" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="K148" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="149" spans="1:11">
@@ -4971,19 +5334,19 @@
         <v>0</v>
       </c>
       <c r="F149" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G149">
         <v>10</v>
       </c>
       <c r="I149" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J149" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="K149" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="150" spans="1:11">
@@ -5003,19 +5366,19 @@
         <v>0</v>
       </c>
       <c r="F150" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G150">
         <v>10</v>
       </c>
       <c r="I150" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J150" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="K150" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="151" spans="1:11">
@@ -5035,22 +5398,22 @@
         <v>0</v>
       </c>
       <c r="F151" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G151">
         <v>10</v>
       </c>
       <c r="H151" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I151" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J151" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="K151" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>